<commit_message>
Risolti problemi di filtraggio e cambiato grafico
Il problema del filtraggio delle commesse era dovuto all'impostazione della data_partenza_veicoli all'anno scorso; la data è stata aggiornata. Il motivo per cui la data è impostata staticamente è che l'istanza è, reale o fittizia che sia, statica; pertanto si imposta così. Sarà necessario renderla dinamica (il codice è già presente ma va "azionato") quando lo schedulatore diverrà reale.
</commit_message>
<xml_diff>
--- a/PS-VRP/INPUT_TEST/MACCHINE12.xlsx
+++ b/PS-VRP/INPUT_TEST/MACCHINE12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wikipedis\Documents\GitHub\progettoIS\PS-VRP\INPUT_TEST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frenc\Documents\GitHub\progettoIS\PS-VRP\INPUT_TEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89077EAF-0CEF-46F1-B138-A739DC711FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4640E63D-BBC8-420C-ABA3-FEC74D78930C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3918BD03-3376-4F28-90D9-48C326B99BD1}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11295" xr2:uid="{3918BD03-3376-4F28-90D9-48C326B99BD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -286,7 +286,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -302,7 +302,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -620,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5669A242-F364-4C2E-83C3-5FEC8505675D}">
   <dimension ref="A1:AN18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2:T18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,7 +1693,7 @@
         <v>55</v>
       </c>
       <c r="B14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1">
         <v>104</v>
@@ -1743,7 +1743,7 @@
         <v>58</v>
       </c>
       <c r="B15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1">
         <v>169</v>
@@ -1793,7 +1793,7 @@
         <v>60</v>
       </c>
       <c r="B16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1">
         <v>195</v>
@@ -1843,7 +1843,7 @@
         <v>62</v>
       </c>
       <c r="B17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1">
         <v>188</v>
@@ -1893,7 +1893,7 @@
         <v>64</v>
       </c>
       <c r="B18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="1">
         <v>146</v>

</xml_diff>

<commit_message>
Aggiustamenti finali 23/04 | primo test commesse
</commit_message>
<xml_diff>
--- a/PS-VRP/INPUT_TEST/MACCHINE12.xlsx
+++ b/PS-VRP/INPUT_TEST/MACCHINE12.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frenc\Documents\GitHub\progettoIS\PS-VRP\INPUT_TEST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wikipedis\Documents\GitHub\progettoIS\PS-VRP\INPUT_TEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4640E63D-BBC8-420C-ABA3-FEC74D78930C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B493FC-845C-4D07-A6CF-69D944F6EC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11295" xr2:uid="{3918BD03-3376-4F28-90D9-48C326B99BD1}"/>
+    <workbookView xWindow="5115" yWindow="2025" windowWidth="15375" windowHeight="7875" xr2:uid="{3918BD03-3376-4F28-90D9-48C326B99BD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -286,7 +286,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -302,7 +302,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -620,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5669A242-F364-4C2E-83C3-5FEC8505675D}">
   <dimension ref="A1:AN18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>